<commit_message>
README update. Creation of audio folder if not yet existent.
</commit_message>
<xml_diff>
--- a/vocabulary.xlsx
+++ b/vocabulary.xlsx
@@ -1,12 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -25,12 +26,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <name val="Calibri"/>
-      <family val="2"/>
       <b val="1"/>
-      <color theme="1"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -50,19 +46,10 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
     </border>
   </borders>
   <cellStyleXfs count="1">
@@ -75,7 +62,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -440,7 +427,7 @@
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -491,6 +478,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>